<commit_message>
Cambios leves calculos y resistencias
</commit_message>
<xml_diff>
--- a/4. CONTROLADOR PID/INFORME PREVIO/calculo_constantes.xlsx
+++ b/4. CONTROLADOR PID/INFORME PREVIO/calculo_constantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\lab-control-i\4. CONTROLADOR PID\INFORME PREVIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\4. CONTROLADOR PID\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D19B07-6F22-4020-9373-8A067C0541DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CAEC2C-CE62-4779-9C31-CE4E089F29CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="13965" windowHeight="16200" activeTab="1" xr2:uid="{06B53DEC-E1BC-4E7F-8CD7-87E0E7A73350}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{06B53DEC-E1BC-4E7F-8CD7-87E0E7A73350}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementación" sheetId="1" r:id="rId1"/>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -259,16 +259,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -276,8 +271,10 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,32 +591,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB54DD9B-6B44-47CF-975E-77E7A4D1A227}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.28515625" customWidth="1"/>
+    <col min="1" max="3" width="8.33203125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" style="18" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="J1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -659,10 +656,7 @@
         <v>440.75</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L4" s="19"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -700,7 +694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>SQRT(C3)</f>
         <v>18.027756377319946</v>
@@ -731,23 +725,23 @@
         <f>0.143-J6</f>
         <v>9.5899999999999985E-2</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="14">
         <v>2</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="13">
         <f>M6*$K$8</f>
         <v>4.886624203821655</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="13">
         <f>$K$10*M6</f>
         <v>51.87499154800058</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="13">
         <f>$K$12*M6</f>
         <v>0.11507999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -773,23 +767,23 @@
       <c r="K7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="17">
         <v>2.5</v>
       </c>
-      <c r="N7" s="20">
+      <c r="N7" s="17">
         <f t="shared" ref="N7:N26" si="3">M7*$K$8</f>
         <v>6.1082802547770685</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="17">
         <f t="shared" ref="O7:O26" si="4">$K$10*M7</f>
         <v>64.843739435000728</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="17">
         <f t="shared" ref="P7:P26" si="5">$K$12*M7</f>
         <v>0.14384999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>B3</f>
         <v>20</v>
@@ -818,41 +812,41 @@
         <f>1.2*K6/J6</f>
         <v>2.4433121019108275</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <v>3</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8">
         <f t="shared" si="3"/>
         <v>7.3299363057324829</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8">
         <f t="shared" si="4"/>
         <v>77.812487322000862</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8">
         <f t="shared" si="5"/>
         <v>0.17262</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="17">
         <v>0.4</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="17">
         <f t="shared" si="0"/>
         <v>4.8000000000000007</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="17">
         <f t="shared" si="1"/>
         <v>27.544382786946329</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="17">
         <f t="shared" si="2"/>
         <v>0.20911704736871958</v>
       </c>
@@ -862,23 +856,23 @@
       <c r="K9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9">
         <v>0.4</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9">
         <f t="shared" si="3"/>
         <v>0.97732484076433102</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9">
         <f t="shared" si="4"/>
         <v>10.374998309600116</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9">
         <f t="shared" si="5"/>
         <v>2.3015999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>0.5*B6</f>
         <v>0.17426420614059965</v>
@@ -887,7 +881,7 @@
         <f>B8/A10</f>
         <v>68.860956967365823</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="15">
         <v>0.04</v>
       </c>
       <c r="E10" s="10">
@@ -910,41 +904,41 @@
         <f>K8/J10</f>
         <v>25.93749577400029</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="12">
         <v>0.04</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10">
         <f t="shared" si="3"/>
         <v>9.7732484076433104E-2</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10">
         <f t="shared" si="4"/>
         <v>1.0374998309600116</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10">
         <f t="shared" si="5"/>
         <v>2.3016E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>0.39</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <f t="shared" si="0"/>
         <v>4.68</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <f t="shared" si="1"/>
         <v>26.85577321727267</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="16">
         <f t="shared" si="2"/>
         <v>0.20388912118450159</v>
       </c>
@@ -954,23 +948,23 @@
       <c r="K11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11">
         <v>0.39</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11">
         <f t="shared" si="3"/>
         <v>0.9528917197452228</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11">
         <f t="shared" si="4"/>
         <v>10.115623351860114</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11">
         <f t="shared" si="5"/>
         <v>2.2440599999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>0.125*B6</f>
         <v>4.3566051535149912E-2</v>
@@ -979,18 +973,18 @@
         <f>B8*A12</f>
         <v>0.52279261842179892</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>0.7</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>8.3999999999999986</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>48.202669877156076</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12">
         <f t="shared" si="2"/>
         <v>0.36595483289525921</v>
       </c>
@@ -1002,471 +996,471 @@
         <f>K8*J12</f>
         <v>5.7539999999999994E-2</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="12">
         <v>0.7</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12">
         <f t="shared" si="3"/>
         <v>1.7103184713375792</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12">
         <f t="shared" si="4"/>
         <v>18.156247041800203</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12">
         <f t="shared" si="5"/>
         <v>4.0277999999999994E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D13" s="14">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D13">
         <v>0.8</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13">
         <f t="shared" ref="E13" si="6">D13*$B$8</f>
         <v>9.6000000000000014</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13">
         <f t="shared" ref="F13" si="7">$B$10*D13</f>
         <v>55.088765573892658</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13">
         <f t="shared" ref="G13" si="8">$B$12*D13</f>
         <v>0.41823409473743917</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13">
         <v>0.8</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13">
         <f t="shared" si="3"/>
         <v>1.954649681528662</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13">
         <f t="shared" si="4"/>
         <v>20.749996619200232</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13">
         <f t="shared" si="5"/>
         <v>4.6031999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D14" s="13">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D14" s="12">
         <v>0.9</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14">
         <f t="shared" ref="E14:E26" si="9">D14*$B$8</f>
         <v>10.8</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14">
         <f t="shared" ref="F14:F20" si="10">$B$10*D14</f>
         <v>61.974861270629241</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14">
         <f t="shared" ref="G14:G20" si="11">$B$12*D14</f>
         <v>0.47051335657961901</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="12">
         <v>0.9</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14">
         <f t="shared" si="3"/>
         <v>2.1989808917197449</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14">
         <f t="shared" si="4"/>
         <v>23.343746196600261</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14">
         <f t="shared" si="5"/>
         <v>5.1785999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D15" s="14">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15">
         <f t="shared" si="10"/>
         <v>68.860956967365823</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15">
         <f t="shared" si="11"/>
         <v>0.52279261842179892</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15">
         <v>1</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15">
         <f t="shared" si="3"/>
         <v>2.4433121019108275</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15">
         <f t="shared" si="4"/>
         <v>25.93749577400029</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15">
         <f t="shared" si="5"/>
         <v>5.7539999999999994E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="13">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D16" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16">
         <f t="shared" si="9"/>
         <v>13.200000000000001</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16">
         <f t="shared" si="10"/>
         <v>75.747052664102412</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16">
         <f t="shared" si="11"/>
         <v>0.57507188026397882</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16">
         <f t="shared" si="3"/>
         <v>2.6876433121019105</v>
       </c>
-      <c r="O16" s="14">
+      <c r="O16">
         <f t="shared" si="4"/>
         <v>28.531245351400322</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16">
         <f t="shared" si="5"/>
         <v>6.3294000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D17" s="14">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D17">
         <v>0.08</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17">
         <f t="shared" si="9"/>
         <v>0.96</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17">
         <f t="shared" si="10"/>
         <v>5.5088765573892662</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17">
         <f t="shared" si="11"/>
         <v>4.1823409473743911E-2</v>
       </c>
-      <c r="M17" s="14">
+      <c r="M17">
         <v>0.08</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17">
         <f t="shared" si="3"/>
         <v>0.19546496815286621</v>
       </c>
-      <c r="O17" s="14">
+      <c r="O17">
         <f t="shared" si="4"/>
         <v>2.0749996619200233</v>
       </c>
-      <c r="P17" s="14">
+      <c r="P17">
         <f t="shared" si="5"/>
         <v>4.6032E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="14">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D18">
         <v>0.04</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18">
         <f t="shared" si="9"/>
         <v>0.48</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18">
         <f t="shared" si="10"/>
         <v>2.7544382786946331</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18">
         <f t="shared" si="11"/>
         <v>2.0911704736871956E-2</v>
       </c>
-      <c r="M18" s="14">
+      <c r="M18">
         <v>0.04</v>
       </c>
-      <c r="N18" s="14">
+      <c r="N18">
         <f t="shared" si="3"/>
         <v>9.7732484076433104E-2</v>
       </c>
-      <c r="O18" s="14">
+      <c r="O18">
         <f t="shared" si="4"/>
         <v>1.0374998309600116</v>
       </c>
-      <c r="P18" s="14">
+      <c r="P18">
         <f t="shared" si="5"/>
         <v>2.3016E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="14">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D19">
         <v>0.1</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19">
         <f t="shared" si="9"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19">
         <f t="shared" si="10"/>
         <v>6.8860956967365823</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19">
         <f t="shared" si="11"/>
         <v>5.2279261842179896E-2</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19">
         <v>0.1</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19">
         <f t="shared" si="3"/>
         <v>0.24433121019108275</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19">
         <f t="shared" si="4"/>
         <v>2.593749577400029</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19">
         <f t="shared" si="5"/>
         <v>5.7539999999999996E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D20" s="14">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D20">
         <v>1.4</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20">
         <f t="shared" si="9"/>
         <v>16.799999999999997</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20">
         <f t="shared" si="10"/>
         <v>96.405339754312152</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20">
         <f t="shared" si="11"/>
         <v>0.73190966579051842</v>
       </c>
-      <c r="M20" s="14">
+      <c r="M20">
         <v>1.4</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20">
         <f t="shared" si="3"/>
         <v>3.4206369426751584</v>
       </c>
-      <c r="O20" s="14">
+      <c r="O20">
         <f t="shared" si="4"/>
         <v>36.312494083600406</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20">
         <f t="shared" si="5"/>
         <v>8.0555999999999989E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D21" s="14">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D21">
         <v>1.5</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21">
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21">
         <f t="shared" ref="F21:F26" si="12">$B$10*D21</f>
         <v>103.29143545104873</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21">
         <f t="shared" ref="G21:G26" si="13">$B$12*D21</f>
         <v>0.78418892763269832</v>
       </c>
-      <c r="M21" s="14">
+      <c r="M21">
         <v>1.5</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21">
         <f t="shared" si="3"/>
         <v>3.6649681528662414</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21">
         <f t="shared" si="4"/>
         <v>38.906243661000431</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21">
         <f t="shared" si="5"/>
         <v>8.6309999999999998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D22" s="14">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D22">
         <v>1.6</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22">
         <f t="shared" si="9"/>
         <v>19.200000000000003</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22">
         <f t="shared" si="12"/>
         <v>110.17753114778532</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22">
         <f t="shared" si="13"/>
         <v>0.83646818947487833</v>
       </c>
-      <c r="M22" s="14">
+      <c r="M22">
         <v>1.6</v>
       </c>
-      <c r="N22" s="14">
+      <c r="N22">
         <f t="shared" si="3"/>
         <v>3.9092993630573241</v>
       </c>
-      <c r="O22" s="14">
+      <c r="O22">
         <f t="shared" si="4"/>
         <v>41.499993238400464</v>
       </c>
-      <c r="P22" s="14">
+      <c r="P22">
         <f t="shared" si="5"/>
         <v>9.2063999999999993E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D23" s="14">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D23">
         <v>1.7</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23">
         <f t="shared" si="9"/>
         <v>20.399999999999999</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23">
         <f t="shared" si="12"/>
         <v>117.06362684452189</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23">
         <f t="shared" si="13"/>
         <v>0.88874745131705812</v>
       </c>
-      <c r="M23" s="14">
+      <c r="M23">
         <v>1.7</v>
       </c>
-      <c r="N23" s="14">
+      <c r="N23">
         <f t="shared" si="3"/>
         <v>4.1536305732484067</v>
       </c>
-      <c r="O23" s="14">
+      <c r="O23">
         <f t="shared" si="4"/>
         <v>44.093742815800489</v>
       </c>
-      <c r="P23" s="14">
+      <c r="P23">
         <f t="shared" si="5"/>
         <v>9.7817999999999988E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D24" s="14">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D24">
         <v>1.8</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24">
         <f t="shared" si="9"/>
         <v>21.6</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24">
         <f t="shared" si="12"/>
         <v>123.94972254125848</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24">
         <f t="shared" si="13"/>
         <v>0.94102671315923803</v>
       </c>
-      <c r="M24" s="14">
+      <c r="M24">
         <v>1.8</v>
       </c>
-      <c r="N24" s="14">
+      <c r="N24">
         <f t="shared" si="3"/>
         <v>4.3979617834394897</v>
       </c>
-      <c r="O24" s="14">
+      <c r="O24">
         <f t="shared" si="4"/>
         <v>46.687492393200522</v>
       </c>
-      <c r="P24" s="14">
+      <c r="P24">
         <f t="shared" si="5"/>
         <v>0.103572</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D25" s="14">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D25">
         <v>1.9</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25">
         <f t="shared" si="9"/>
         <v>22.799999999999997</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25">
         <f t="shared" si="12"/>
         <v>130.83581823799506</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25">
         <f t="shared" si="13"/>
         <v>0.99330597500141793</v>
       </c>
-      <c r="M25" s="14">
+      <c r="M25">
         <v>1.9</v>
       </c>
-      <c r="N25" s="14">
+      <c r="N25">
         <f t="shared" si="3"/>
         <v>4.6422929936305719</v>
       </c>
-      <c r="O25" s="14">
+      <c r="O25">
         <f t="shared" si="4"/>
         <v>49.281241970600547</v>
       </c>
-      <c r="P25" s="14">
+      <c r="P25">
         <f t="shared" si="5"/>
         <v>0.10932599999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D26" s="14">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26">
         <f t="shared" si="9"/>
         <v>24</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26">
         <f t="shared" si="12"/>
         <v>137.72191393473165</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26">
         <f t="shared" si="13"/>
         <v>1.0455852368435978</v>
       </c>
-      <c r="M26" s="14">
+      <c r="M26">
         <v>2</v>
       </c>
-      <c r="N26" s="14">
+      <c r="N26">
         <f t="shared" si="3"/>
         <v>4.886624203821655</v>
       </c>
-      <c r="O26" s="14">
+      <c r="O26">
         <f t="shared" si="4"/>
         <v>51.87499154800058</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26">
         <f t="shared" si="5"/>
         <v>0.11507999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1504,45 +1498,45 @@
         <v>0.14384999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N29" s="22" t="s">
+      <c r="N29" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="P29" s="22" t="s">
+      <c r="P29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="22" t="s">
+      <c r="Q29" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <f>1*10^3</f>
         <v>1000</v>
@@ -1586,12 +1580,12 @@
         <f>$Q$28/Q30</f>
         <v>14384.999999999998</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="Q30">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>330</v>
       </c>
@@ -1611,7 +1605,7 @@
         <f t="shared" ref="G31:G41" si="16">$H$28/H31</f>
         <v>9500</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
@@ -1639,7 +1633,7 @@
         <v>2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1684,7 +1678,7 @@
         <v>4.6999999999999997E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B33">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1726,7 +1720,7 @@
         <v>9.9999999999999991E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1768,7 +1762,7 @@
         <v>4.6999999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B35">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1778,7 +1772,7 @@
         <v>3630.5547487656113</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E31:E41" si="20">10*10^-6</f>
+        <f t="shared" ref="E35:E41" si="20">10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="G35">
@@ -1786,7 +1780,7 @@
         <v>4446.8085106382978</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H33:H41" si="21">47*10^-6</f>
+        <f t="shared" ref="H35:H41" si="21">47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="K35">
@@ -1810,7 +1804,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B36">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1840,7 +1834,7 @@
         <v>1542.1865120367659</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N31:N41" si="22">10*10^-6</f>
+        <f t="shared" ref="N36:N41" si="22">10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="P36">
@@ -1852,7 +1846,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B37">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1894,7 +1888,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B38">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1936,7 +1930,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B39">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1978,7 +1972,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B40">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -2020,7 +2014,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B41">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -2062,7 +2056,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>22</v>
       </c>
@@ -2094,25 +2088,25 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="14">
+      <c r="B45">
         <f>E43*$B$8</f>
         <v>7.1999999999999993</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45">
         <f>$B$10*E43</f>
         <v>41.316574180419494</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45">
         <v>0.1</v>
       </c>
       <c r="J45" s="1" t="s">
@@ -2136,45 +2130,45 @@
         <v>0.14384999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="22" t="s">
+      <c r="E46" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="G46" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J46" s="22" t="s">
+      <c r="J46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K46" s="22" t="s">
+      <c r="K46" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M46" s="22" t="s">
+      <c r="M46" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N46" s="22" t="s">
+      <c r="N46" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="P46" s="22" t="s">
+      <c r="P46" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Q46" s="22" t="s">
+      <c r="Q46" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>100</v>
       </c>
@@ -2205,11 +2199,11 @@
         <f>$K$45*J47/$K$43</f>
         <v>851.063829787234</v>
       </c>
-      <c r="M47" s="19">
+      <c r="M47">
         <f>$K$43/($N$45*N47)</f>
         <v>7248.1939520333699</v>
       </c>
-      <c r="N47" s="19">
+      <c r="N47">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
@@ -2222,8 +2216,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>220</v>
       </c>
       <c r="B48">
@@ -2238,15 +2232,15 @@
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="G48" s="19">
+      <c r="G48">
         <f t="shared" ref="G48:G58" si="25">$H$45/($B$43*H48)</f>
         <v>967.11798839458413</v>
       </c>
-      <c r="H48" s="19">
+      <c r="H48">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="J48" s="19">
+      <c r="J48">
         <v>220</v>
       </c>
       <c r="K48">
@@ -2261,51 +2255,51 @@
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="P48" s="19">
+      <c r="P48">
         <f t="shared" ref="P48:P58" si="28">$Q$45/($K$43*Q48)</f>
         <v>1391.199226305609</v>
       </c>
-      <c r="Q48" s="19">
+      <c r="Q48">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="19">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>330</v>
       </c>
-      <c r="B49" s="19">
-        <f t="shared" ref="B48:B65" si="29">$B$45*A49/$B$43</f>
+      <c r="B49">
+        <f t="shared" ref="B49:B65" si="29">$B$45*A49/$B$43</f>
         <v>505.53191489361689</v>
       </c>
-      <c r="D49" s="19">
+      <c r="D49">
         <f t="shared" si="24"/>
         <v>2420.3361963972179</v>
       </c>
-      <c r="E49" s="19">
+      <c r="E49">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="G49" s="19">
+      <c r="G49">
         <f t="shared" si="25"/>
         <v>452.69352648257131</v>
       </c>
-      <c r="H49" s="19">
+      <c r="H49">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="J49" s="19">
+      <c r="J49">
         <v>330</v>
       </c>
       <c r="K49">
         <f t="shared" si="26"/>
         <v>2808.5106382978724</v>
       </c>
-      <c r="M49" s="19">
+      <c r="M49">
         <f t="shared" si="27"/>
         <v>1542.1689259645468</v>
       </c>
-      <c r="N49" s="19">
+      <c r="N49">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
@@ -2313,24 +2307,24 @@
         <f t="shared" si="28"/>
         <v>651.1996378451787</v>
       </c>
-      <c r="Q49" s="19">
+      <c r="Q49">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="19">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>750</v>
       </c>
-      <c r="B50" s="19">
+      <c r="B50">
         <f t="shared" si="29"/>
         <v>1148.9361702127658</v>
       </c>
-      <c r="D50" s="19">
+      <c r="D50">
         <f t="shared" si="24"/>
         <v>1137.5580123066925</v>
       </c>
-      <c r="E50" s="19">
+      <c r="E50">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
@@ -2338,18 +2332,18 @@
         <f t="shared" si="25"/>
         <v>212.76595744680853</v>
       </c>
-      <c r="H50" s="19">
+      <c r="H50">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="J50" s="19">
+      <c r="J50">
         <v>750</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50">
         <f t="shared" si="26"/>
         <v>6382.9787234042551</v>
       </c>
-      <c r="M50" s="19">
+      <c r="M50">
         <f t="shared" si="27"/>
         <v>724.81939520333708</v>
       </c>
@@ -2366,7 +2360,7 @@
         <v>9.9999999999999991E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>1000</v>
       </c>
@@ -2390,14 +2384,14 @@
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
-      <c r="J51" s="19">
+      <c r="J51">
         <v>1000</v>
       </c>
-      <c r="K51" s="19">
+      <c r="K51">
         <f t="shared" si="26"/>
         <v>8510.6382978723395</v>
       </c>
-      <c r="M51" s="19">
+      <c r="M51">
         <f t="shared" si="27"/>
         <v>154.21689259645467</v>
       </c>
@@ -2414,8 +2408,8 @@
         <v>4.6999999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="19">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>1200</v>
       </c>
       <c r="B52">
@@ -2438,14 +2432,14 @@
         <f t="shared" ref="H52:H58" si="31">47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="J52" s="19">
+      <c r="J52">
         <v>1200</v>
       </c>
       <c r="K52">
         <f t="shared" si="26"/>
         <v>10212.765957446809</v>
       </c>
-      <c r="M52" s="19">
+      <c r="M52">
         <f t="shared" si="27"/>
         <v>72.481939520333697</v>
       </c>
@@ -2462,8 +2456,8 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="19">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>1800</v>
       </c>
       <c r="B53">
@@ -2486,14 +2480,14 @@
         <f t="shared" si="31"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="J53" s="19">
+      <c r="J53">
         <v>1800</v>
       </c>
       <c r="K53">
         <f t="shared" si="26"/>
         <v>15319.148936170212</v>
       </c>
-      <c r="M53" s="19">
+      <c r="M53">
         <f t="shared" si="27"/>
         <v>7248.1939520333699</v>
       </c>
@@ -2510,8 +2504,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="19">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>2000</v>
       </c>
       <c r="B54">
@@ -2534,14 +2528,14 @@
         <f t="shared" si="31"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="J54" s="19">
+      <c r="J54">
         <v>2000</v>
       </c>
       <c r="K54">
         <f t="shared" si="26"/>
         <v>17021.276595744679</v>
       </c>
-      <c r="M54" s="19">
+      <c r="M54">
         <f t="shared" si="27"/>
         <v>7248.1939520333699</v>
       </c>
@@ -2558,8 +2552,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="19">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>2200</v>
       </c>
       <c r="B55">
@@ -2582,14 +2576,14 @@
         <f t="shared" si="31"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="J55" s="19">
+      <c r="J55">
         <v>2200</v>
       </c>
       <c r="K55">
         <f t="shared" si="26"/>
         <v>18723.404255319147</v>
       </c>
-      <c r="M55" s="19">
+      <c r="M55">
         <f t="shared" si="27"/>
         <v>7248.1939520333699</v>
       </c>
@@ -2606,8 +2600,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="19">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56">
         <v>560</v>
       </c>
       <c r="B56">
@@ -2637,7 +2631,7 @@
         <f t="shared" si="26"/>
         <v>4765.9574468085102</v>
       </c>
-      <c r="M56" s="19">
+      <c r="M56">
         <f t="shared" si="27"/>
         <v>7248.1939520333699</v>
       </c>
@@ -2654,8 +2648,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="19">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>820</v>
       </c>
       <c r="B57">
@@ -2678,14 +2672,14 @@
         <f t="shared" si="31"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="J57" s="19">
+      <c r="J57">
         <v>820</v>
       </c>
       <c r="K57">
         <f t="shared" si="26"/>
         <v>6978.7234042553191</v>
       </c>
-      <c r="M57" s="19">
+      <c r="M57">
         <f t="shared" si="27"/>
         <v>7248.1939520333699</v>
       </c>
@@ -2702,7 +2696,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B58">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -2724,10 +2718,10 @@
         <v>4.6999999999999997E-5</v>
       </c>
       <c r="K58">
-        <f t="shared" ref="K48:K58" si="34">$K$28*J58/$K$43</f>
-        <v>0</v>
-      </c>
-      <c r="M58" s="19">
+        <f t="shared" ref="K58" si="34">$K$28*J58/$K$43</f>
+        <v>0</v>
+      </c>
+      <c r="M58">
         <f t="shared" si="27"/>
         <v>7248.1939520333699</v>
       </c>
@@ -2744,45 +2738,45 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B59">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B61">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B63">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B64">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -2802,29 +2796,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F877A2-64C7-4558-925C-765001584139}">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G25" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView topLeftCell="I37" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="12" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2834,7 +2828,7 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2845,7 +2839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2855,7 +2849,7 @@
       <c r="C3">
         <v>65</v>
       </c>
-      <c r="I3" s="21"/>
+      <c r="I3" s="18"/>
       <c r="J3">
         <v>1</v>
       </c>
@@ -2866,11 +2860,10 @@
         <v>215.25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I4" s="21"/>
-      <c r="L4" s="19"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2889,7 +2882,7 @@
       <c r="G5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="18"/>
       <c r="J5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2909,7 +2902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>SQRT(C3)</f>
         <v>8.0622577482985491</v>
@@ -2918,22 +2911,22 @@
         <f>2*PI()/A6</f>
         <v>0.77933322195083421</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>0.1</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6">
         <f t="shared" ref="E6:E26" si="0">D6*$B$8</f>
         <v>0.12</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6">
         <f t="shared" ref="F6:F26" si="1">$B$10*D6</f>
         <v>0.30795556154943554</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6">
         <f t="shared" ref="G6:G26" si="2">$B$12*D6</f>
         <v>1.1689998329262513E-2</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="18"/>
       <c r="J6" s="5">
         <v>1.9400000000000001E-2</v>
       </c>
@@ -2941,66 +2934,66 @@
         <f>0.2122-J6</f>
         <v>0.1928</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="24">
         <v>2</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="17">
         <f>M6*$K$8</f>
         <v>23.851546391752574</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="17">
         <f>$K$10*M6</f>
         <v>614.73057710702506</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="17">
         <f>$K$12*M6</f>
         <v>0.23135999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7">
         <v>0.2</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7">
         <f t="shared" si="1"/>
         <v>0.61591112309887108</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7">
         <f t="shared" si="2"/>
         <v>2.3379996658525026E-2</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="4"/>
       <c r="K7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="27">
+      <c r="M7">
         <v>2.5</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7">
         <f t="shared" ref="N7:N26" si="3">M7*$K$8</f>
         <v>29.814432989690719</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7">
         <f t="shared" ref="O7:O26" si="4">$K$10*M7</f>
         <v>768.41322138378132</v>
       </c>
-      <c r="P7" s="27">
+      <c r="P7">
         <f t="shared" ref="P7:P26" si="5">$K$12*M7</f>
         <v>0.28919999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>B3</f>
         <v>2</v>
@@ -3009,89 +3002,89 @@
         <f>0.6*A8</f>
         <v>1.2</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>0.3</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8">
         <f t="shared" si="1"/>
         <v>0.92386668464830646</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8">
         <f t="shared" si="2"/>
         <v>3.5069994987787539E-2</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="5"/>
       <c r="K8" s="7">
         <f>1.2*K6/J6</f>
         <v>11.925773195876287</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <v>3</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8">
         <f t="shared" si="3"/>
         <v>35.77731958762886</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8">
         <f t="shared" si="4"/>
         <v>922.09586566053758</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8">
         <f t="shared" si="5"/>
         <v>0.34703999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>0.4</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <f t="shared" si="1"/>
         <v>1.2318222461977422</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <f t="shared" si="2"/>
         <v>4.6759993317050053E-2</v>
       </c>
-      <c r="I9" s="21"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9">
         <v>0.4</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9">
         <f t="shared" si="3"/>
         <v>4.7703092783505152</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9">
         <f t="shared" si="4"/>
         <v>122.94611542140501</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9">
         <f t="shared" si="5"/>
         <v>4.6272000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>0.5*B6</f>
         <v>0.3896666109754171</v>
@@ -3100,22 +3093,22 @@
         <f>B8/A10</f>
         <v>3.0795556154943551</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <v>0.04</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10">
         <f t="shared" si="1"/>
         <v>0.12318222461977421</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10">
         <f t="shared" si="2"/>
         <v>4.6759993317050056E-3</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="5">
         <f>2*J6</f>
         <v>3.8800000000000001E-2</v>
@@ -3124,68 +3117,68 @@
         <f>K8/J10</f>
         <v>307.36528855351253</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="12">
         <v>0.04</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10">
         <f t="shared" si="3"/>
         <v>0.47703092783505152</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10">
         <f t="shared" si="4"/>
         <v>12.294611542140501</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10">
         <f t="shared" si="5"/>
         <v>4.6271999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11">
         <v>0.39</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>0.46799999999999997</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11">
         <f t="shared" si="1"/>
         <v>1.2010266900427986</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11">
         <f t="shared" si="2"/>
         <v>4.55909934841238E-2</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11">
         <v>0.39</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11">
         <f t="shared" si="3"/>
         <v>4.6510515463917521</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11">
         <f t="shared" si="4"/>
         <v>119.87246253586989</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11">
         <f t="shared" si="5"/>
         <v>4.5115200000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>0.125*B6</f>
         <v>9.7416652743854276E-2</v>
@@ -3194,22 +3187,22 @@
         <f>B8*A12</f>
         <v>0.11689998329262513</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>0.7</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>0.84</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>2.1556889308460483</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12">
         <f t="shared" si="2"/>
         <v>8.1829988304837592E-2</v>
       </c>
-      <c r="I12" s="21"/>
+      <c r="I12" s="18"/>
       <c r="J12" s="5">
         <f>0.5*J6</f>
         <v>9.7000000000000003E-3</v>
@@ -3218,488 +3211,488 @@
         <f>K8*J12</f>
         <v>0.11567999999999999</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="12">
         <v>0.7</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12">
         <f t="shared" si="3"/>
         <v>8.3480412371134012</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12">
         <f t="shared" si="4"/>
         <v>215.15570198745877</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12">
         <f t="shared" si="5"/>
         <v>8.0975999999999992E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D13" s="14">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D13">
         <v>0.8</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13">
         <f t="shared" si="1"/>
         <v>2.4636444923954843</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13">
         <f t="shared" si="2"/>
         <v>9.3519986634100105E-2</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="M13" s="14">
+      <c r="I13" s="18"/>
+      <c r="M13">
         <v>0.8</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13">
         <f t="shared" si="3"/>
         <v>9.5406185567010304</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13">
         <f t="shared" si="4"/>
         <v>245.89223084281002</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13">
         <f t="shared" si="5"/>
         <v>9.2544000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D14" s="13">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D14" s="12">
         <v>0.9</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14">
         <f t="shared" si="1"/>
         <v>2.7716000539449195</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14">
         <f t="shared" si="2"/>
         <v>0.10520998496336262</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="M14" s="13">
+      <c r="I14" s="18"/>
+      <c r="M14" s="12">
         <v>0.9</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14">
         <f t="shared" si="3"/>
         <v>10.733195876288658</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14">
         <f t="shared" si="4"/>
         <v>276.62875969816128</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14">
         <f t="shared" si="5"/>
         <v>0.104112</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D15" s="14">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15">
         <f t="shared" si="1"/>
         <v>3.0795556154943551</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15">
         <f t="shared" si="2"/>
         <v>0.11689998329262513</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="M15" s="14">
+      <c r="I15" s="18"/>
+      <c r="M15">
         <v>1</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15">
         <f t="shared" si="3"/>
         <v>11.925773195876287</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15">
         <f t="shared" si="4"/>
         <v>307.36528855351253</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15">
         <f t="shared" si="5"/>
         <v>0.11567999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="24">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D16" s="21">
         <v>1.2</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <f t="shared" si="0"/>
         <v>1.44</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <f t="shared" si="1"/>
         <v>3.6954667385932258</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="22">
         <f t="shared" si="2"/>
         <v>0.14027997995115016</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="M16" s="13">
+      <c r="I16" s="18"/>
+      <c r="M16" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16">
         <f t="shared" si="3"/>
         <v>13.118350515463916</v>
       </c>
-      <c r="O16" s="14">
+      <c r="O16">
         <f t="shared" si="4"/>
         <v>338.10181740886378</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16">
         <f t="shared" si="5"/>
         <v>0.127248</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D17" s="25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D17" s="22">
         <v>2</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="22">
         <f t="shared" si="1"/>
         <v>6.1591112309887102</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="22">
         <f t="shared" si="2"/>
         <v>0.23379996658525026</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="M17" s="14">
+      <c r="I17" s="18"/>
+      <c r="M17">
         <v>0.08</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17">
         <f t="shared" si="3"/>
         <v>0.95406185567010304</v>
       </c>
-      <c r="O17" s="14">
+      <c r="O17">
         <f t="shared" si="4"/>
         <v>24.589223084281002</v>
       </c>
-      <c r="P17" s="14">
+      <c r="P17">
         <f t="shared" si="5"/>
         <v>9.2543999999999994E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D18" s="25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D18" s="22">
         <v>2.5</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="22">
         <f t="shared" si="1"/>
         <v>7.6988890387358877</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="22">
         <f t="shared" si="2"/>
         <v>0.29224995823156286</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="M18" s="14">
+      <c r="I18" s="18"/>
+      <c r="M18">
         <v>0.04</v>
       </c>
-      <c r="N18" s="14">
+      <c r="N18">
         <f t="shared" si="3"/>
         <v>0.47703092783505152</v>
       </c>
-      <c r="O18" s="14">
+      <c r="O18">
         <f t="shared" si="4"/>
         <v>12.294611542140501</v>
       </c>
-      <c r="P18" s="14">
+      <c r="P18">
         <f t="shared" si="5"/>
         <v>4.6271999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D19" s="25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D19" s="22">
         <v>5</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="22">
         <f t="shared" si="1"/>
         <v>15.397778077471775</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="22">
         <f t="shared" si="2"/>
         <v>0.58449991646312571</v>
       </c>
-      <c r="I19" s="21"/>
-      <c r="M19" s="14">
+      <c r="I19" s="18"/>
+      <c r="M19">
         <v>0.1</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19">
         <f t="shared" si="3"/>
         <v>1.1925773195876288</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19">
         <f t="shared" si="4"/>
         <v>30.736528855351253</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19">
         <f t="shared" si="5"/>
         <v>1.1568E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D20" s="26">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D20" s="23">
         <v>10</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="23">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="23">
         <f t="shared" si="1"/>
         <v>30.795556154943551</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="23">
         <f t="shared" si="2"/>
         <v>1.1689998329262514</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="M20" s="14">
+      <c r="I20" s="18"/>
+      <c r="M20">
         <v>1.4</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20">
         <f t="shared" si="3"/>
         <v>16.696082474226802</v>
       </c>
-      <c r="O20" s="14">
+      <c r="O20">
         <f t="shared" si="4"/>
         <v>430.31140397491754</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20">
         <f t="shared" si="5"/>
         <v>0.16195199999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D21" s="14">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D21">
         <v>12.5</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21">
         <f t="shared" si="1"/>
         <v>38.494445193679439</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21">
         <f t="shared" si="2"/>
         <v>1.4612497911578142</v>
       </c>
-      <c r="I21" s="21"/>
-      <c r="M21" s="14">
+      <c r="I21" s="18"/>
+      <c r="M21">
         <v>1.5</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21">
         <f t="shared" si="3"/>
         <v>17.88865979381443</v>
       </c>
-      <c r="O21" s="14">
+      <c r="O21">
         <f t="shared" si="4"/>
         <v>461.04793283026879</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21">
         <f t="shared" si="5"/>
         <v>0.17351999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D22" s="26">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D22" s="23">
         <v>15</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="23">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="23">
         <f t="shared" si="1"/>
         <v>46.193334232415324</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="23">
         <f t="shared" si="2"/>
         <v>1.7534997493893769</v>
       </c>
-      <c r="I22" s="21"/>
-      <c r="M22" s="14">
+      <c r="I22" s="18"/>
+      <c r="M22">
         <v>1.6</v>
       </c>
-      <c r="N22" s="14">
+      <c r="N22">
         <f t="shared" si="3"/>
         <v>19.081237113402061</v>
       </c>
-      <c r="O22" s="14">
+      <c r="O22">
         <f t="shared" si="4"/>
         <v>491.78446168562004</v>
       </c>
-      <c r="P22" s="14">
+      <c r="P22">
         <f t="shared" si="5"/>
         <v>0.185088</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D23" s="14">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D23">
         <v>17.5</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23">
         <f t="shared" si="1"/>
         <v>53.892223271151217</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23">
         <f t="shared" si="2"/>
         <v>2.0457497076209399</v>
       </c>
-      <c r="I23" s="21"/>
-      <c r="M23" s="14">
+      <c r="I23" s="18"/>
+      <c r="M23">
         <v>1.7</v>
       </c>
-      <c r="N23" s="14">
+      <c r="N23">
         <f t="shared" si="3"/>
         <v>20.273814432989688</v>
       </c>
-      <c r="O23" s="14">
+      <c r="O23">
         <f t="shared" si="4"/>
         <v>522.5209905409713</v>
       </c>
-      <c r="P23" s="14">
+      <c r="P23">
         <f t="shared" si="5"/>
         <v>0.19665599999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D24" s="15">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D24" s="13">
         <v>20</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="13">
         <f t="shared" si="1"/>
         <v>61.591112309887102</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="13">
         <f t="shared" si="2"/>
         <v>2.3379996658525029</v>
       </c>
-      <c r="I24" s="21"/>
-      <c r="M24" s="14">
+      <c r="I24" s="18"/>
+      <c r="M24">
         <v>1.8</v>
       </c>
-      <c r="N24" s="14">
+      <c r="N24">
         <f t="shared" si="3"/>
         <v>21.466391752577316</v>
       </c>
-      <c r="O24" s="14">
+      <c r="O24">
         <f t="shared" si="4"/>
         <v>553.25751939632255</v>
       </c>
-      <c r="P24" s="14">
+      <c r="P24">
         <f t="shared" si="5"/>
         <v>0.20822399999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D25" s="20">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D25" s="17">
         <v>22.5</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="17">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="17">
         <f t="shared" si="1"/>
         <v>69.290001348622994</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="17">
         <f t="shared" si="2"/>
         <v>2.6302496240840654</v>
       </c>
-      <c r="I25" s="21"/>
-      <c r="M25" s="14">
+      <c r="I25" s="18"/>
+      <c r="M25">
         <v>1.9</v>
       </c>
-      <c r="N25" s="14">
+      <c r="N25">
         <f t="shared" si="3"/>
         <v>22.658969072164943</v>
       </c>
-      <c r="O25" s="14">
+      <c r="O25">
         <f t="shared" si="4"/>
         <v>583.9940482516738</v>
       </c>
-      <c r="P25" s="14">
+      <c r="P25">
         <f t="shared" si="5"/>
         <v>0.21979199999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D26" s="14">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D26">
         <v>25</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26">
         <f t="shared" si="1"/>
         <v>76.988890387358879</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26">
         <f t="shared" si="2"/>
         <v>2.9224995823156283</v>
       </c>
-      <c r="I26" s="21"/>
-      <c r="M26" s="14">
+      <c r="I26" s="18"/>
+      <c r="M26">
         <v>2</v>
       </c>
-      <c r="N26" s="14">
+      <c r="N26">
         <f t="shared" si="3"/>
         <v>23.851546391752574</v>
       </c>
-      <c r="O26" s="14">
+      <c r="O26">
         <f t="shared" si="4"/>
         <v>614.73057710702506</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26">
         <f t="shared" si="5"/>
         <v>0.23135999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I27" s="21"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -3718,7 +3711,7 @@
       <c r="H28">
         <v>0.20899999999999999</v>
       </c>
-      <c r="I28" s="21"/>
+      <c r="I28" s="18"/>
       <c r="J28" s="1" t="s">
         <v>10</v>
       </c>
@@ -3738,46 +3731,46 @@
         <v>0.14384999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="21"/>
-      <c r="J29" s="22" t="s">
+      <c r="I29" s="18"/>
+      <c r="J29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="22" t="s">
+      <c r="K29" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N29" s="22" t="s">
+      <c r="N29" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="P29" s="22" t="s">
+      <c r="P29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="22" t="s">
+      <c r="Q29" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <f>1*10^3</f>
         <v>1000</v>
@@ -3802,7 +3795,7 @@
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="I30" s="21"/>
+      <c r="I30" s="18"/>
       <c r="J30">
         <v>100</v>
       </c>
@@ -3822,12 +3815,12 @@
         <f>$Q$28/Q30</f>
         <v>14384.999999999998</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="Q30">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>330</v>
       </c>
@@ -3847,11 +3840,11 @@
         <f t="shared" ref="G31:G41" si="8">$H$28/H31</f>
         <v>9500</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="I31" s="21"/>
+      <c r="I31" s="18"/>
       <c r="J31">
         <v>220</v>
       </c>
@@ -3876,7 +3869,7 @@
         <v>2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3897,7 +3890,7 @@
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I32" s="21"/>
+      <c r="I32" s="18"/>
       <c r="J32" s="1">
         <v>330</v>
       </c>
@@ -3922,7 +3915,7 @@
         <v>4.6999999999999997E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B33">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3943,7 +3936,7 @@
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="I33" s="21"/>
+      <c r="I33" s="18"/>
       <c r="K33">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -3965,7 +3958,7 @@
         <v>9.9999999999999991E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3986,7 +3979,7 @@
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
-      <c r="I34" s="21"/>
+      <c r="I34" s="18"/>
       <c r="K34">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4008,7 +4001,7 @@
         <v>4.6999999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B35">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4018,7 +4011,7 @@
         <v>3630.5547487656113</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E45" si="12">10*10^-6</f>
+        <f t="shared" ref="E35:E41" si="12">10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="G35">
@@ -4026,10 +4019,10 @@
         <v>4446.8085106382978</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H43" si="13">47*10^-6</f>
+        <f t="shared" ref="H35:H41" si="13">47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I35" s="21"/>
+      <c r="I35" s="18"/>
       <c r="K35">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4051,7 +4044,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B36">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4072,7 +4065,7 @@
         <f t="shared" si="13"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I36" s="21"/>
+      <c r="I36" s="18"/>
       <c r="K36">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4082,7 +4075,7 @@
         <v>1542.1865120367659</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36:N46" si="14">10*10^-6</f>
+        <f t="shared" ref="N36:N41" si="14">10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="P36">
@@ -4094,7 +4087,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B37">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4115,7 +4108,7 @@
         <f t="shared" si="13"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I37" s="21"/>
+      <c r="I37" s="18"/>
       <c r="K37">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4137,7 +4130,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B38">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4158,7 +4151,7 @@
         <f t="shared" si="13"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I38" s="21"/>
+      <c r="I38" s="18"/>
       <c r="K38">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4180,7 +4173,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B39">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4201,7 +4194,7 @@
         <f t="shared" si="13"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I39" s="21"/>
+      <c r="I39" s="18"/>
       <c r="K39">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4223,7 +4216,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B40">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4244,7 +4237,7 @@
         <f t="shared" si="13"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I40" s="21"/>
+      <c r="I40" s="18"/>
       <c r="K40">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4266,7 +4259,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B41">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4287,7 +4280,7 @@
         <f t="shared" si="13"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I41" s="21"/>
+      <c r="I41" s="18"/>
       <c r="K41">
         <f t="shared" si="9"/>
         <v>0</v>
@@ -4309,10 +4302,10 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I42" s="21"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>22</v>
       </c>
@@ -4328,7 +4321,7 @@
       <c r="E43">
         <v>25</v>
       </c>
-      <c r="I43" s="21"/>
+      <c r="I43" s="18"/>
       <c r="J43" s="1" t="s">
         <v>22</v>
       </c>
@@ -4345,31 +4338,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I44" s="21"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I44" s="18"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="14">
+      <c r="B45">
         <f>E43*$B$8</f>
         <v>30</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45">
         <f>$B$10*E43</f>
         <v>76.988890387358879</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I45" s="21"/>
+      <c r="I45" s="18"/>
       <c r="J45" s="1" t="s">
         <v>10</v>
       </c>
@@ -4392,46 +4385,46 @@
         <v>0.23135999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="22" t="s">
+      <c r="E46" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="G46" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="22" t="s">
+      <c r="I46" s="18"/>
+      <c r="J46" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K46" s="22" t="s">
+      <c r="K46" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M46" s="22" t="s">
+      <c r="M46" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N46" s="22" t="s">
+      <c r="N46" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="P46" s="22" t="s">
+      <c r="P46" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="Q46" s="22" t="s">
+      <c r="Q46" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>100</v>
       </c>
@@ -4447,15 +4440,15 @@
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="G47" s="19">
+      <c r="G47">
         <f>$H$45/($B$43*H47)</f>
         <v>11702.127659574469</v>
       </c>
-      <c r="H47" s="19">
+      <c r="H47">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="I47" s="21"/>
+      <c r="I47" s="18"/>
       <c r="J47">
         <v>100</v>
       </c>
@@ -4463,28 +4456,28 @@
         <f>$K$45*J47/$K$43</f>
         <v>761.21956569423105</v>
       </c>
-      <c r="M47" s="19">
+      <c r="M47">
         <f>$K$43/($N$45*N47)</f>
         <v>764.56258644536683</v>
       </c>
-      <c r="N47" s="19">
+      <c r="N47">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="P47" s="19">
+      <c r="P47">
         <f>$Q$45/($K$43*Q47)</f>
         <v>4922.5531914893618</v>
       </c>
-      <c r="Q47" s="19">
+      <c r="Q47">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>220</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48">
         <f>$B$45*A48/$B$43</f>
         <v>1404.2553191489362</v>
       </c>
@@ -4496,15 +4489,15 @@
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="G48" s="19">
+      <c r="G48">
         <f t="shared" ref="G48:G58" si="17">$H$45/($B$43*H48)</f>
         <v>5319.1489361702124</v>
       </c>
-      <c r="H48" s="19">
+      <c r="H48">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="I48" s="21"/>
+      <c r="I48" s="18"/>
       <c r="J48" s="1">
         <v>220</v>
       </c>
@@ -4520,52 +4513,52 @@
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="P48" s="19">
+      <c r="P48">
         <f t="shared" ref="P48:P58" si="20">$Q$45/($K$43*Q48)</f>
         <v>2237.5241779497096</v>
       </c>
-      <c r="Q48" s="19">
+      <c r="Q48">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="19">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>330</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49">
         <f t="shared" ref="B49:B58" si="21">$B$45*A49/$B$43</f>
         <v>2106.382978723404</v>
       </c>
-      <c r="D49" s="19">
+      <c r="D49">
         <f t="shared" si="16"/>
         <v>1298.8887032513903</v>
       </c>
-      <c r="E49" s="19">
+      <c r="E49">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="G49" s="19">
+      <c r="G49">
         <f t="shared" si="17"/>
         <v>2489.8143956541421</v>
       </c>
-      <c r="H49" s="19">
+      <c r="H49">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I49" s="21"/>
-      <c r="J49" s="19">
+      <c r="I49" s="18"/>
+      <c r="J49">
         <v>330</v>
       </c>
-      <c r="K49" s="19">
+      <c r="K49">
         <f t="shared" si="18"/>
         <v>2512.0245667909621</v>
       </c>
-      <c r="M49" s="19">
+      <c r="M49">
         <f t="shared" si="19"/>
         <v>162.67289073305676</v>
       </c>
-      <c r="N49" s="19">
+      <c r="N49">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
@@ -4578,7 +4571,7 @@
         <v>4.6999999999999997E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>750</v>
       </c>
@@ -4586,11 +4579,11 @@
         <f t="shared" si="21"/>
         <v>4787.2340425531911</v>
       </c>
-      <c r="D50" s="19">
+      <c r="D50">
         <f t="shared" si="16"/>
         <v>610.47769052815352</v>
       </c>
-      <c r="E50" s="19">
+      <c r="E50">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
@@ -4602,36 +4595,36 @@
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="I50" s="21"/>
-      <c r="J50" s="19">
+      <c r="I50" s="18"/>
+      <c r="J50">
         <v>750</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50">
         <f t="shared" si="18"/>
         <v>5709.1467427067328</v>
       </c>
-      <c r="M50" s="19">
+      <c r="M50">
         <f t="shared" si="19"/>
         <v>76.456258644536675</v>
       </c>
-      <c r="N50" s="19">
+      <c r="N50">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="P50" s="19">
+      <c r="P50">
         <f t="shared" si="20"/>
         <v>492.25531914893617</v>
       </c>
-      <c r="Q50" s="19">
+      <c r="Q50">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="19">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>1000</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51">
         <f t="shared" si="21"/>
         <v>6382.9787234042551</v>
       </c>
@@ -4643,23 +4636,23 @@
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
-      <c r="G51" s="19">
+      <c r="G51">
         <f t="shared" si="17"/>
         <v>248.98143956541423</v>
       </c>
-      <c r="H51" s="19">
+      <c r="H51">
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
-      <c r="I51" s="21"/>
-      <c r="J51" s="19">
+      <c r="I51" s="18"/>
+      <c r="J51">
         <v>1000</v>
       </c>
-      <c r="K51" s="19">
+      <c r="K51">
         <f t="shared" si="18"/>
         <v>7612.1956569423101</v>
       </c>
-      <c r="M51" s="19">
+      <c r="M51">
         <f t="shared" si="19"/>
         <v>16.267289073305676</v>
       </c>
@@ -4676,8 +4669,8 @@
         <v>4.6999999999999999E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="19">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>1200</v>
       </c>
       <c r="B52">
@@ -4700,15 +4693,15 @@
         <f>1000*10^-6</f>
         <v>1E-3</v>
       </c>
-      <c r="I52" s="21"/>
-      <c r="J52" s="19">
+      <c r="I52" s="18"/>
+      <c r="J52">
         <v>1200</v>
       </c>
       <c r="K52">
         <f t="shared" si="18"/>
         <v>9134.6347883307717</v>
       </c>
-      <c r="M52" s="19">
+      <c r="M52">
         <f t="shared" si="19"/>
         <v>7.6456258644536677</v>
       </c>
@@ -4725,8 +4718,8 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="19">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>1800</v>
       </c>
       <c r="B53">
@@ -4746,18 +4739,18 @@
         <v>2489.8143956541421</v>
       </c>
       <c r="H53">
-        <f t="shared" ref="H52:H58" si="23">47*10^-6</f>
+        <f t="shared" ref="H53:H58" si="23">47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I53" s="21"/>
-      <c r="J53" s="19">
+      <c r="I53" s="18"/>
+      <c r="J53">
         <v>1800</v>
       </c>
       <c r="K53">
         <f t="shared" si="18"/>
         <v>13701.952182496159</v>
       </c>
-      <c r="M53" s="19">
+      <c r="M53">
         <f t="shared" si="19"/>
         <v>764.56258644536683</v>
       </c>
@@ -4774,8 +4767,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="19">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>2000</v>
       </c>
       <c r="B54">
@@ -4798,15 +4791,15 @@
         <f t="shared" si="23"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I54" s="21"/>
-      <c r="J54" s="19">
+      <c r="I54" s="18"/>
+      <c r="J54">
         <v>2000</v>
       </c>
       <c r="K54">
         <f t="shared" si="18"/>
         <v>15224.39131388462</v>
       </c>
-      <c r="M54" s="19">
+      <c r="M54">
         <f t="shared" si="19"/>
         <v>764.56258644536683</v>
       </c>
@@ -4823,8 +4816,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="19">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>2200</v>
       </c>
       <c r="B55">
@@ -4847,15 +4840,15 @@
         <f t="shared" si="23"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I55" s="21"/>
-      <c r="J55" s="19">
+      <c r="I55" s="18"/>
+      <c r="J55">
         <v>2200</v>
       </c>
       <c r="K55">
         <f t="shared" si="18"/>
         <v>16746.830445273084</v>
       </c>
-      <c r="M55" s="19">
+      <c r="M55">
         <f t="shared" si="19"/>
         <v>764.56258644536683</v>
       </c>
@@ -4872,8 +4865,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="19">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56">
         <v>560</v>
       </c>
       <c r="B56">
@@ -4896,15 +4889,15 @@
         <f t="shared" si="23"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I56" s="21"/>
-      <c r="J56" s="19">
+      <c r="I56" s="18"/>
+      <c r="J56">
         <v>560</v>
       </c>
-      <c r="K56" s="19">
+      <c r="K56">
         <f t="shared" si="18"/>
         <v>4262.8295678876939</v>
       </c>
-      <c r="M56" s="19">
+      <c r="M56">
         <f t="shared" si="19"/>
         <v>764.56258644536683</v>
       </c>
@@ -4921,8 +4914,8 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="19">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>820</v>
       </c>
       <c r="B57">
@@ -4945,15 +4938,15 @@
         <f t="shared" si="23"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I57" s="21"/>
-      <c r="J57" s="19">
+      <c r="I57" s="18"/>
+      <c r="J57">
         <v>820</v>
       </c>
       <c r="K57">
         <f t="shared" si="18"/>
         <v>6242.0004386926939</v>
       </c>
-      <c r="M57" s="19">
+      <c r="M57">
         <f t="shared" si="19"/>
         <v>764.56258644536683</v>
       </c>
@@ -4970,7 +4963,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B58">
         <f t="shared" si="21"/>
         <v>0</v>
@@ -4991,12 +4984,12 @@
         <f t="shared" si="23"/>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="I58" s="21"/>
+      <c r="I58" s="18"/>
       <c r="K58">
         <f t="shared" ref="K58" si="26">$K$28*J58/$K$43</f>
         <v>0</v>
       </c>
-      <c r="M58" s="19">
+      <c r="M58">
         <f t="shared" si="19"/>
         <v>764.56258644536683</v>
       </c>

</xml_diff>